<commit_message>
'update report PD BE'
</commit_message>
<xml_diff>
--- a/tx_backend_pd_dc_0p7_0p42_Feb26_tsmc2ff_meas.xlsx
+++ b/tx_backend_pd_dc_0p7_0p42_Feb26_tsmc2ff_meas.xlsx
@@ -331,7 +331,7 @@
     <t>0.700</t>
   </si>
   <si>
-    <t>0.420</t>
+    <t>0.450</t>
   </si>
   <si>
     <t>0.750</t>
@@ -376,7 +376,7 @@
     <t>0.735</t>
   </si>
   <si>
-    <t>0.441</t>
+    <t>0.473</t>
   </si>
   <si>
     <t>0.770</t>
@@ -394,7 +394,7 @@
     <t>tsmc2ff (3)</t>
   </si>
   <si>
-    <t>0.3864</t>
+    <t>0.414</t>
   </si>
   <si>
     <t>0.630</t>

</xml_diff>